<commit_message>
[API] Crea y recupera pedidos correctamente
</commit_message>
<xml_diff>
--- a/api/Documentacion/Rutas.xlsx
+++ b/api/Documentacion/Rutas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PROGRAMACION\Projecte-final-2DAM\api\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7501259-18F0-4444-B181-9BD04785F11B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ED88672-BAA9-478E-A0DC-B0796FF63809}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17160" yWindow="2604" windowWidth="11376" windowHeight="8928" xr2:uid="{8A5A3C78-CEDF-4A18-8457-A6EDB3924A20}"/>
+    <workbookView xWindow="17316" yWindow="3036" windowWidth="11376" windowHeight="8928" xr2:uid="{8A5A3C78-CEDF-4A18-8457-A6EDB3924A20}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -676,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3E054A7-B27E-4442-AE88-B16BFCD81E8F}">
   <dimension ref="A3:I95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -790,7 +790,7 @@
       <c r="A11" t="s">
         <v>75</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -1369,7 +1369,7 @@
     </row>
     <row r="73" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B73" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
[API] Documentacion, mejoras de codigo y arreglado errores
</commit_message>
<xml_diff>
--- a/api/Documentacion/Rutas.xlsx
+++ b/api/Documentacion/Rutas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PROGRAMACION\Projecte-final-2DAM\api\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C480B1-DF19-49A6-9F22-A0A0E99C511C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B9D068-DDDC-47E6-ACBA-D7D4AECDD182}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9084" yWindow="1572" windowWidth="11376" windowHeight="8928" xr2:uid="{8A5A3C78-CEDF-4A18-8457-A6EDB3924A20}"/>
+    <workbookView xWindow="11664" yWindow="3432" windowWidth="11376" windowHeight="8928" xr2:uid="{8A5A3C78-CEDF-4A18-8457-A6EDB3924A20}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="145">
   <si>
     <t>Usuario</t>
   </si>
@@ -237,12 +237,6 @@
     <t>tienda/{id}/pedido/{id}/favorito</t>
   </si>
   <si>
-    <t>Listar pedidos favoritos de una tienda</t>
-  </si>
-  <si>
-    <t>Añadir un pedido de una tienda a favoritos</t>
-  </si>
-  <si>
     <t>Registrar-se</t>
   </si>
   <si>
@@ -334,9 +328,6 @@
   </si>
   <si>
     <t>Eliminar producto tienda propia</t>
-  </si>
-  <si>
-    <t>Crear nuevo producto tienda propia</t>
   </si>
   <si>
     <t>Ver categorias tienda propia</t>
@@ -500,6 +491,27 @@
   </si>
   <si>
     <t>tokens</t>
+  </si>
+  <si>
+    <t>Añadir producto base a tienda propia</t>
+  </si>
+  <si>
+    <t>Crear producto especifico en tienda</t>
+  </si>
+  <si>
+    <t>Añadir</t>
+  </si>
+  <si>
+    <t>Productos (Base)</t>
+  </si>
+  <si>
+    <t>Listar productos base</t>
+  </si>
+  <si>
+    <t>productos/base</t>
+  </si>
+  <si>
+    <t>Listar productos especificos</t>
   </si>
 </sst>
 </file>
@@ -910,10 +922,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3E054A7-B27E-4442-AE88-B16BFCD81E8F}">
-  <dimension ref="A3:I111"/>
+  <dimension ref="A3:I113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -946,15 +958,15 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>1</v>
@@ -963,7 +975,7 @@
         <v>18</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -971,7 +983,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>2</v>
@@ -988,7 +1000,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>3</v>
@@ -1002,36 +1014,36 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>20</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -1041,10 +1053,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>6</v>
@@ -1058,10 +1070,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>4</v>
@@ -1080,10 +1092,10 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>5</v>
@@ -1097,10 +1109,10 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>7</v>
@@ -1114,10 +1126,10 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>8</v>
@@ -1136,10 +1148,10 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>5</v>
@@ -1153,10 +1165,10 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>7</v>
@@ -1165,15 +1177,15 @@
         <v>18</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>8</v>
@@ -1199,10 +1211,10 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>5</v>
@@ -1216,10 +1228,10 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>6</v>
@@ -1233,10 +1245,10 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>7</v>
@@ -1250,7 +1262,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>13</v>
@@ -1267,7 +1279,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>13</v>
@@ -1278,32 +1290,35 @@
       <c r="D32" s="5" t="s">
         <v>28</v>
       </c>
+      <c r="E32" s="3" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>18</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B36" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>5</v>
@@ -1312,12 +1327,12 @@
         <v>20</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>6</v>
@@ -1326,7 +1341,7 @@
         <v>20</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
@@ -1340,12 +1355,12 @@
         <v>18</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>4</v>
@@ -1354,12 +1369,12 @@
         <v>19</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>8</v>
@@ -1368,7 +1383,7 @@
         <v>28</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -1381,10 +1396,10 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>6</v>
@@ -1398,10 +1413,10 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>7</v>
@@ -1415,10 +1430,10 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>4</v>
@@ -1432,7 +1447,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>13</v>
@@ -1454,10 +1469,10 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>5</v>
@@ -1471,7 +1486,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>13</v>
@@ -1488,13 +1503,13 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>101</v>
+        <v>138</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>7</v>
+        <v>140</v>
       </c>
       <c r="D53" s="5" t="s">
         <v>18</v>
@@ -1505,128 +1520,131 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>99</v>
+        <v>139</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B55" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B57" s="4" t="s">
-        <v>54</v>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>98</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>102</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>50</v>
+        <v>99</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C60" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B61" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C61" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D60" s="5" t="s">
+      <c r="D61" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E60" s="3" t="s">
+      <c r="E61" s="3" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B62" s="4" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>109</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D63" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E63" s="3" t="s">
-        <v>57</v>
+        <v>106</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B64" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>57</v>
@@ -1634,16 +1652,16 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B65" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>57</v>
@@ -1651,353 +1669,365 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B66" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B68" s="4" t="s">
-        <v>59</v>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B67" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>111</v>
-      </c>
-      <c r="B69" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>60</v>
+        <v>108</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B70" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D70" s="5" t="s">
         <v>20</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B71" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B76" s="4" t="s">
-        <v>47</v>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B72" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>113</v>
-      </c>
-      <c r="B77" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D77" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E77" s="3" t="s">
-        <v>17</v>
+        <v>110</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C78" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B79" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C79" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D78" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E78" s="3" t="s">
+      <c r="D79" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E79" s="3" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B80" s="4" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>115</v>
-      </c>
-      <c r="B81" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D81" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E81" s="3" t="s">
-        <v>26</v>
+        <v>112</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C82" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B83" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C83" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D82" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E82" s="3" t="s">
+      <c r="D83" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E83" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B83" s="6"/>
-    </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B84" s="4" t="s">
-        <v>62</v>
-      </c>
+      <c r="B84" s="6"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>117</v>
-      </c>
-      <c r="B85" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C85" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B86" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C86" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D85" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E85" s="3" t="s">
+      <c r="D86" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E86" s="3" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B87" s="4" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>105</v>
-      </c>
-      <c r="B88" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C88" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B89" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C89" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D88" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E88" s="3" t="s">
+      <c r="D89" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E89" s="3" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B90" s="4" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>118</v>
-      </c>
-      <c r="B91" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C91" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D91" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E91" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F91" s="3" t="s">
-        <v>120</v>
+        <v>115</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="B92" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C92" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D92" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E92" s="12" t="s">
-        <v>33</v>
+        <v>116</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D92" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E92" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F92" s="3" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>121</v>
-      </c>
-      <c r="B93" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C93" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D93" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E93" s="3" t="s">
-        <v>35</v>
+        <v>118</v>
+      </c>
+      <c r="B93" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C93" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D93" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E93" s="12" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="B94" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C94" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D94" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E94" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="F94" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
+      </c>
+      <c r="B94" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D94" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E94" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" s="8" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B95" s="9" t="s">
         <v>13</v>
       </c>
       <c r="C95" s="10" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D95" s="9" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="E95" s="10" t="s">
         <v>33</v>
       </c>
       <c r="F95" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B96" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C96" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D96" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E96" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F96" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>123</v>
+      </c>
+      <c r="B98" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>124</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D99" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E99" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B97" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
-        <v>126</v>
-      </c>
-      <c r="B98" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C98" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D98" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E98" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
-        <v>127</v>
-      </c>
-      <c r="B99" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C99" s="3" t="s">
+      <c r="B100" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C100" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D99" s="5" t="s">
+      <c r="D100" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E99" s="3" t="s">
+      <c r="E100" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B102" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B103" s="5" t="s">
-        <v>80</v>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>142</v>
       </c>
       <c r="C103" s="3" t="s">
         <v>5</v>
@@ -2006,35 +2036,55 @@
         <v>20</v>
       </c>
       <c r="E103" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>144</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D104" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B111" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B112" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D112" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E112" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B104" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C104" s="3" t="s">
+    <row r="113" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B113" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C113" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D104" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E104" s="3" t="s">
+      <c r="D113" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E113" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F110" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F111" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="63" fitToWidth="0" fitToHeight="0" pageOrder="overThenDown" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>